<commit_message>
Schematic updates. First export to PCB
Added 9V line, OLED switch circuit. Added OLED footprint.
</commit_message>
<xml_diff>
--- a/Hardware/remote_shutter_controller/BOM.xlsx
+++ b/Hardware/remote_shutter_controller/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor Tamarin\Documents\GitHub\Canon-Intervalometer\Hardware\remote_shutter_controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB9992A-8BC3-4B52-BAAD-D7417805F1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B31D90-5446-4947-9DDB-E73A82E6E755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12030" yWindow="4185" windowWidth="22275" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Part</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>X077-6428TSWCG01-H13</t>
+  </si>
+  <si>
+    <t>78L09-150 UMW(Youtai Semiconductor Co., Ltd.) | C347271 - LCSC Electronics</t>
+  </si>
+  <si>
+    <t>9V LDO</t>
+  </si>
+  <si>
+    <t>78L09-150</t>
   </si>
 </sst>
 </file>
@@ -254,8 +263,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}" name="Table1" displayName="Table1" ref="A1:F15" totalsRowShown="0">
-  <autoFilter ref="A1:F15" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}" name="Table1" displayName="Table1" ref="A1:F16" totalsRowShown="0">
+  <autoFilter ref="A1:F16" xr:uid="{4009DC08-B675-4320-8612-FFC6D25BDBAE}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9964CAF8-BC40-4857-A93B-37018EB66BEB}" name="Part"/>
     <tableColumn id="2" xr3:uid="{759936DF-FAE0-45E5-B671-94997451E316}" name="Description"/>
@@ -533,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,6 +870,27 @@
       </c>
       <c r="F15" s="1" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.43</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -879,11 +909,12 @@
     <hyperlink ref="F14" r:id="rId12" display="https://www.lcsc.com/product-detail/Slide-Switches_G-Switch-MK-12D18-G020_C3019727.html" xr:uid="{E838C8F8-4747-4AE5-B5C6-0AABD0F5FF38}"/>
     <hyperlink ref="F15" r:id="rId13" display="https://www.lcsc.com/product-detail/Battery-Management-ICs_TPOWER-TP4056_C382139.html" xr:uid="{111A80ED-4D8C-4F2E-A3B2-170394732200}"/>
     <hyperlink ref="F6" r:id="rId14" display="https://www.lcsc.com/product-detail/span-style-background-color-ff0-OLED-span-Displays-Modules_Shenzhen-Allvision-Tech-X077-6428TSWCG01-H13_C5123562.html" xr:uid="{82996C4F-131B-4FEB-B6FA-DD3201D5991B}"/>
+    <hyperlink ref="F16" r:id="rId15" display="https://www.lcsc.com/product-detail/Linear-Voltage-Regulators-LDO_UMW-Youtai-Semiconductor-Co-Ltd-78L09-150_C347271.html" xr:uid="{033E9E82-1730-442B-B54E-769F5D1A2A55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
   <tableParts count="1">
-    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>